<commit_message>
add some parts to the excel sheets and mark them green in Scratch list of parts
</commit_message>
<xml_diff>
--- a/Forms/ნაწილების სია(AutoRecovered).xlsx
+++ b/Forms/ნაწილების სია(AutoRecovered).xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\alex\senjorpraeqt\Senior_Project_BB-8\Forms\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\x1_user\Desktop\Semester 7\Senior_Project_BB-8\Forms\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA73C70E-89B3-4624-B5A8-7936638BB47D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="2085" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="2090" windowWidth="15380" windowHeight="7880"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
-  <si>
-    <t>Column6</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="64">
   <si>
     <t>Column7</t>
   </si>
@@ -51,9 +47,6 @@
     <t>რაოდენობა</t>
   </si>
   <si>
-    <t>ფასი</t>
-  </si>
-  <si>
     <t>esp-32</t>
   </si>
   <si>
@@ -142,13 +135,94 @@
   </si>
   <si>
     <t>https://detail.tmall.com/item.htm?abbucket=8&amp;id=764789305038&amp;ns=1&amp;pisk=g5Sq3h2sToE4S4s4sLxZY5qHdWxvNnVQ0GO6IOXMhIADGOvMb_f_HI6gM1SwZOQbHFNxQxIPTcibMrBibhtgOWZQAtpvXhVITedEWjpedxq6ocmkDdTYN8G7AtBv6xlgdaqI_GAgvj0Ms1xkrdvwjKADju2yQpRMjIYiZ0vBZCxGsEmorpvKSKAMnT2yKpiiic0DZTvBImcGsh2PEQpiwnSGArp9oRvmapZzCzQWttArjDlJeEcFQVioqgJDuGfeaL954K82TUwn44scNOjfDUUxlhB5817Gt7gXiwJFae_4Tm5FMdfkEswsWL7NIMKvkAi1Tn5w-iYrIDWHmQKyEM2sJQsyG1j2rJie53jB-nb7yST60p5GDskZj6X5diLRbWlk6Z9pqdSTKVRwSgJr6LqdVGQqsV8DeLRQU8Sqe5bAOdfgGV39kLpyO-cSWVLDeLRQU8utWEGpUBwmN&amp;priceTId=2100c80817362542227243176e0960&amp;skuId=5433658427577&amp;spm=a21n57.1.item.51.3246523cmKNB97&amp;utparam=%7B%22aplus_abtest%22%3A%2225ea0f96550d55c38f3daae8b6dd9529%22%7D&amp;xxc=taobaoSearch</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>ceramic capacitors</t>
+  </si>
+  <si>
+    <t>常用独石电容器直插50V无极陶瓷电容10 102 104 105 106混装套件-tmall.com天猫</t>
+  </si>
+  <si>
+    <t>მეოთხე (4)  - 10 ნაირი, თითო 30 ცალი</t>
+  </si>
+  <si>
+    <t>ressistors</t>
+  </si>
+  <si>
+    <t>盒装1/4W金属膜电阻器 直插五色环电阻包 精度1% 30种600个元件包-tmall.com天猫</t>
+  </si>
+  <si>
+    <t>ფასი (უანი)</t>
+  </si>
+  <si>
+    <t>盒装1/4w金属膜电阻包 精度1% 30种常用直插五色环电阻包 共600只-淘宝网</t>
+  </si>
+  <si>
+    <t>electrolytic capacitors</t>
+  </si>
+  <si>
+    <t>包邮 15种规格200个铝电解电容器分类盒套件 范围0.1uF - 220uF-淘宝网</t>
+  </si>
+  <si>
+    <t>LEDs</t>
+  </si>
+  <si>
+    <t>200个3mm发光二极管灯珠LED灯珠直插5种色白/红/黄/绿/蓝混装盒装-tmall.com天猫</t>
+  </si>
+  <si>
+    <t>彩色电路板飞线 单芯镀锡铜线 航空线 八色OK线 跳线 8色电子导线-淘宝网</t>
+  </si>
+  <si>
+    <t>breadboard tin wires</t>
+  </si>
+  <si>
+    <t>盒装14种长度140根优质跳线面包板线面包板专用线面包板跳线560根-tmall.com天猫</t>
+  </si>
+  <si>
+    <t>DIY电线美标1007电子线镀锡铜16AWG-30AWG 五色5卷彩盒装电路配线-tmall.com天猫</t>
+  </si>
+  <si>
+    <t>thick copper cables</t>
+  </si>
+  <si>
+    <t>think copper cables</t>
+  </si>
+  <si>
+    <t>26 AWG 5 rolls 20m - red, black, yellow, blue, green</t>
+  </si>
+  <si>
+    <t>(工厂直销)微型导电滑环帽式信号集电环无人机手持云台稳拍器锚鱼-tmall.com天猫</t>
+  </si>
+  <si>
+    <t>HM012-08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slip ring with 8 cores </t>
+  </si>
+  <si>
+    <t>4 cores - (2)</t>
+  </si>
+  <si>
+    <t>HM007-04</t>
+  </si>
+  <si>
+    <t>https://detail.tmall.com/item.htm?abbucket=16&amp;id=696738835325&amp;ns=1&amp;priceTId=2100c81917362611679056275e0c0f&amp;skuId=5113669519438&amp;spm=a21n57.1.item.10.3ab2523cgB5l4r&amp;utparam=%7B%22aplus_abtest%22%3A%22823e5f90a423abd75b708fb7a287d995%22%7D&amp;xxc=taobaoSearch</t>
+  </si>
+  <si>
+    <t>牛眼轮滚珠万向球CY-15-25A加厚钢球尼龙球不锈钢一寸牛眼轴承-淘宝网</t>
+  </si>
+  <si>
+    <t>ball transfer unit</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -159,6 +233,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF11192D"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,17 +263,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -208,19 +293,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{A9721D4D-F39B-4758-AC29-175E2C175F17}" name="Table1" displayName="Table1" ref="C3:L36" totalsRowShown="0">
-  <autoFilter ref="C3:L36" xr:uid="{51834E56-920C-49D8-B3CF-EEC68D9F15FB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="C3:L36" totalsRowShown="0">
+  <autoFilter ref="C3:L36"/>
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{04473FB6-833B-4D4D-A363-2BBD9D03AFC3}" name="დასახელება"/>
-    <tableColumn id="2" xr3:uid="{47E0DB59-5840-49B2-A5C1-31B11AAA2E3A}" name="აღწერა"/>
-    <tableColumn id="3" xr3:uid="{76447349-697D-4147-96DA-A3A237211631}" name="ლინკი"/>
-    <tableColumn id="4" xr3:uid="{8A079DA6-02FA-46F0-91E0-1C0924D54E95}" name="რაოდენობა"/>
-    <tableColumn id="5" xr3:uid="{A4519058-19A1-40F4-AB2E-8EA85815968D}" name="ფასი"/>
-    <tableColumn id="6" xr3:uid="{1DA6A1E4-CD17-416C-94F0-D25D422E7E77}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{55C84997-E99E-4B6B-A66A-347F915B464B}" name="Column7"/>
-    <tableColumn id="8" xr3:uid="{FA68113E-DE2E-4CBE-945C-05EDD7A52CA3}" name="Column8"/>
-    <tableColumn id="9" xr3:uid="{7583B644-4517-4E1F-BC01-9AB0AC6E115A}" name="Column9"/>
-    <tableColumn id="10" xr3:uid="{9B257CD0-4D92-4CB9-B82F-78E66262CA40}" name="Column10"/>
+    <tableColumn id="1" name="დასახელება"/>
+    <tableColumn id="2" name="აღწერა"/>
+    <tableColumn id="3" name="ლინკი"/>
+    <tableColumn id="4" name="რაოდენობა"/>
+    <tableColumn id="5" name="ფასი (უანი)"/>
+    <tableColumn id="6" name="Column1"/>
+    <tableColumn id="7" name="Column7"/>
+    <tableColumn id="8" name="Column8"/>
+    <tableColumn id="9" name="Column9"/>
+    <tableColumn id="10" name="Column10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium27" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -488,195 +573,377 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:L13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C3:L26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B9" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="28.7109375" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" customWidth="1"/>
-    <col min="5" max="11" width="11" customWidth="1"/>
+    <col min="3" max="3" width="28.7265625" customWidth="1"/>
+    <col min="4" max="4" width="38.90625" customWidth="1"/>
+    <col min="5" max="5" width="22.6328125" customWidth="1"/>
+    <col min="6" max="6" width="8.6328125" customWidth="1"/>
+    <col min="7" max="7" width="12.90625" customWidth="1"/>
+    <col min="8" max="11" width="11" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>1</v>
+      </c>
+      <c r="K3" t="s">
+        <v>2</v>
+      </c>
+      <c r="L3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" t="s">
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" t="s">
-        <v>1</v>
-      </c>
-      <c r="J3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" t="s">
-        <v>3</v>
-      </c>
-      <c r="L3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>10</v>
-      </c>
-      <c r="E4" t="s">
-        <v>12</v>
       </c>
       <c r="F4">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" t="s">
+        <v>13</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C6" t="s">
         <v>14</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
-        <v>13</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
+      <c r="F6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" t="s">
+    </row>
+    <row r="7" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" t="s">
         <v>17</v>
-      </c>
-      <c r="F6" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" t="s">
-        <v>19</v>
       </c>
       <c r="F7">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
         <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" t="s">
-        <v>24</v>
       </c>
       <c r="F8">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
         <v>25</v>
       </c>
-      <c r="D9" t="s">
-        <v>27</v>
-      </c>
       <c r="E9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F9">
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:12" x14ac:dyDescent="0.35">
       <c r="C10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" t="s">
         <v>29</v>
       </c>
-      <c r="D10" t="s">
-        <v>30</v>
-      </c>
-      <c r="E10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="F11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D12" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
         <v>32</v>
       </c>
-      <c r="D11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="F12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:12" ht="29" x14ac:dyDescent="0.35">
+      <c r="C13" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" t="s">
         <v>31</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C12" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E12" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="3:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="C13" s="2" t="s">
+      <c r="E13" t="s">
         <v>36</v>
       </c>
-      <c r="D13" t="s">
-        <v>33</v>
-      </c>
-      <c r="E13" t="s">
+      <c r="F13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="3:12" x14ac:dyDescent="0.35">
+      <c r="C16" t="s">
         <v>38</v>
       </c>
-      <c r="F13">
-        <v>1</v>
+      <c r="D16" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>15.3</v>
+      </c>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C17" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>8.5</v>
+      </c>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C18" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C21" t="s">
+        <v>54</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C22" t="s">
+        <v>50</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>6.8</v>
+      </c>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C23" t="s">
+        <v>53</v>
+      </c>
+      <c r="D23" t="s">
+        <v>55</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C24" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" t="s">
+        <v>59</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>19.5</v>
+      </c>
+    </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s">
+        <v>58</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>28.5</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.35">
+      <c r="C26" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F26">
+        <v>10</v>
+      </c>
+      <c r="G26">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E16" r:id="rId1" display="https://detail.tmall.com/item.htm?abbucket=16&amp;id=683034367107&amp;ns=1&amp;priceTId=2100c88b17362582914603827e0b9b&amp;skuId=5059393567466&amp;spm=a21n57.1.hoverItem.18&amp;utparam=%7B%22aplus_abtest%22%3A%22dbef30766743e9bdc0908690cab7e10d%22%7D&amp;xxc=taobaoSearch"/>
+    <hyperlink ref="E17" r:id="rId2" display="https://detail.tmall.com/item.htm?abbucket=19&amp;id=683328413168&amp;rn=896644150738fdb84b70fe3ad1f2f6a8&amp;spm=a312a.7700824.w4011-24536307509.23.492f4fcbUPCvnq"/>
+    <hyperlink ref="E18" r:id="rId3" display="https://item.taobao.com/item.htm?abbucket=16&amp;id=692606109403&amp;ns=1&amp;priceTId=2100c82617362588475892273e0bdb&amp;skuId=4920392277588&amp;spm=a21n57.1.hoverItem.3&amp;utparam=%7B%22aplus_abtest%22%3A%2235eaa792299d844b1d713e490844695b%22%7D&amp;xxc=taobaoSearch"/>
+    <hyperlink ref="E19" r:id="rId4" display="https://item.taobao.com/item.htm?id=590356028467&amp;spm=a312a.7700824.w4002-17890096034.10.34ae360073nLf5"/>
+    <hyperlink ref="E20" r:id="rId5" display="https://detail.tmall.com/item.htm?abbucket=19&amp;id=688719980119&amp;rn=eade812c00e43e1a6fe078681dafec5f&amp;spm=a312a.7700824.w4011-24536280695.17.747d1d6cCstSrI"/>
+    <hyperlink ref="E21" r:id="rId6" display="https://item.taobao.com/item.htm?abbucket=16&amp;id=561340834902&amp;ns=1&amp;priceTId=2100c82017362598290412075e0c3a&amp;spm=a21n57.1.hoverItem.10&amp;utparam=%7B%22aplus_abtest%22%3A%2237473e2815a2142aca576aafb856b6de%22%7D&amp;xxc=taobaoSearch&amp;skuId=3681678599166"/>
+    <hyperlink ref="E22" r:id="rId7" display="https://detail.tmall.com/item.htm?abbucket=16&amp;id=669570807944&amp;ns=1&amp;priceTId=2100c82017362601420764632e0c3a&amp;skuId=4816986937763&amp;spm=a21n57.1.hoverItem.8&amp;utparam=%7B%22aplus_abtest%22%3A%22e0d86be345cedc12a9bf1d1670ffddf5%22%7D&amp;xxc=taobaoSearch"/>
+    <hyperlink ref="E23" r:id="rId8" display="https://detail.tmall.com/item.htm?abbucket=16&amp;id=748642438763&amp;ns=1&amp;priceTId=2100c82017362603051832136e0c3a&amp;skuId=5330660182434&amp;spm=a21n57.1.hoverItem.15&amp;utparam=%7B%22aplus_abtest%22%3A%2215d36f0d173efbdc83a936c085f0c4b4%22%7D&amp;xxc=taobaoSearch"/>
+    <hyperlink ref="E25" r:id="rId9" display="https://detail.tmall.com/item.htm?abbucket=16&amp;id=696738835325&amp;ns=1&amp;priceTId=2100c81917362611679056275e0c0f&amp;skuId=5218038054222&amp;spm=a21n57.1.item.10.3ab2523cgB5l4r&amp;utparam=%7B%22aplus_abtest%22%3A%22823e5f90a423abd75b708fb7a287d995%22%7D&amp;xxc=taobaoSearch"/>
+    <hyperlink ref="E24" r:id="rId10"/>
+    <hyperlink ref="E26" r:id="rId11" display="https://item.taobao.com/item.htm?from=cart&amp;id=632591281487&amp;skuId=4985800979644&amp;spm=a1z0d.6639537%2F202410.item.d632591281487.3d387182fv6OId"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId12"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId13"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>